<commit_message>
Beleza funcionou agora adicionar para pegar o Preço Médio e o Código Fipe
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -1,22 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.vinicius\Documents\Vscode\Fipe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABC8E2-29E5-4321-9D59-228DF70EB656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+  <si>
+    <t>MarcaSelecionada</t>
+  </si>
+  <si>
+    <t>ModeloSelecionado</t>
+  </si>
+  <si>
+    <t>AnoSelecionado</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>Agrale</t>
+  </si>
+  <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>Integra GS 1.8</t>
+  </si>
+  <si>
+    <t>Legend 3.2/3.5</t>
+  </si>
+  <si>
+    <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
+  </si>
+  <si>
+    <t>MARRUÁ AM 100 2.8  CS TDI Diesel</t>
+  </si>
+  <si>
+    <t>145 Elegant 1.7/1.8 16V</t>
+  </si>
+  <si>
+    <t>145 Elegant 2.0 16V</t>
+  </si>
+  <si>
+    <t>1992 Gasolina</t>
+  </si>
+  <si>
+    <t>1991 Gasolina</t>
+  </si>
+  <si>
+    <t>1998 Gasolina</t>
+  </si>
+  <si>
+    <t>1997 Gasolina</t>
+  </si>
+  <si>
+    <t>2007 Diesel</t>
+  </si>
+  <si>
+    <t>2006 Diesel</t>
+  </si>
+  <si>
+    <t>1999 Gasolina</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,25 +116,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -96,7 +198,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -130,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -164,9 +267,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -339,13 +443,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Consegui pegar agora arrumar para pegar todos os modelos e Ano de determinada Marca
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.vinicius\Documents\Vscode\Fipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABC8E2-29E5-4321-9D59-228DF70EB656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3E6A1D-1748-4679-9F3A-56E892A57E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -31,6 +31,12 @@
     <t>AnoSelecionado</t>
   </si>
   <si>
+    <t>CodigoFipe</t>
+  </si>
+  <si>
+    <t>PrecoMedio</t>
+  </si>
+  <si>
     <t>Acura</t>
   </si>
   <si>
@@ -77,6 +83,51 @@
   </si>
   <si>
     <t>1999 Gasolina</t>
+  </si>
+  <si>
+    <t>038003-2</t>
+  </si>
+  <si>
+    <t>038002-4</t>
+  </si>
+  <si>
+    <t>060001-6</t>
+  </si>
+  <si>
+    <t>006009-7</t>
+  </si>
+  <si>
+    <t>006001-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11120.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10387.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14248.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 48348.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44601.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43449.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27043.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21667.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21690.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17716.00</t>
   </si>
 </sst>
 </file>
@@ -444,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,9 +506,11 @@
     <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,137 +520,215 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arrumei a forma como pegar o código e o preço médio
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -37,7 +37,76 @@
     <t>Integra GS 1.8</t>
   </si>
   <si>
+    <t>Legend 3.2/3.5</t>
+  </si>
+  <si>
+    <t>NSX 3.0</t>
+  </si>
+  <si>
     <t>1992 Gasolina</t>
+  </si>
+  <si>
+    <t>1991 Gasolina</t>
+  </si>
+  <si>
+    <t>1998 Gasolina</t>
+  </si>
+  <si>
+    <t>1997 Gasolina</t>
+  </si>
+  <si>
+    <t>1996 Gasolina</t>
+  </si>
+  <si>
+    <t>1995 Gasolina</t>
+  </si>
+  <si>
+    <t>1994 Gasolina</t>
+  </si>
+  <si>
+    <t>1993 Gasolina</t>
+  </si>
+  <si>
+    <t>038003-2</t>
+  </si>
+  <si>
+    <t>038002-4</t>
+  </si>
+  <si>
+    <t>038001-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11097.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10366.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25397.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22580.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19084.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14802.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14219.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40991.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39550.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36538.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33397.00</t>
   </si>
 </sst>
 </file>
@@ -395,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +495,251 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug do Scroll arrumado - Solução fazer Limpar a pesquisa sempre que for pegar outro Ano Modelo
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
   <si>
     <t>MarcaSelecionada</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Acura</t>
   </si>
   <si>
+    <t>Agrale</t>
+  </si>
+  <si>
     <t>Integra GS 1.8</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t>NSX 3.0</t>
   </si>
   <si>
+    <t>MARRUÁ 2.8 12V 132cv TDI Diesel</t>
+  </si>
+  <si>
     <t>1992 Gasolina</t>
   </si>
   <si>
@@ -67,13 +73,31 @@
     <t>1993 Gasolina</t>
   </si>
   <si>
+    <t>2007 Diesel</t>
+  </si>
+  <si>
+    <t>2006 Diesel</t>
+  </si>
+  <si>
+    <t>2005 Diesel</t>
+  </si>
+  <si>
+    <t>2004 Diesel</t>
+  </si>
+  <si>
     <t>038003-2</t>
   </si>
   <si>
+    <t>038001-6</t>
+  </si>
+  <si>
     <t>038002-4</t>
   </si>
   <si>
-    <t>038001-6</t>
+    <t>006009-7</t>
+  </si>
+  <si>
+    <t>060001-6</t>
   </si>
   <si>
     <t xml:space="preserve"> 11097.00</t>
@@ -82,31 +106,52 @@
     <t xml:space="preserve"> 10366.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 25397.00</t>
+    <t xml:space="preserve"> 40991.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 22580.00</t>
   </si>
   <si>
+    <t xml:space="preserve"> 21233.00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 19084.00</t>
   </si>
   <si>
+    <t xml:space="preserve"> 18267.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16282.00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 14802.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 14219.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 40991.00</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 39550.00</t>
   </si>
   <si>
+    <t xml:space="preserve"> 38236.00</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 36538.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 33397.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27313.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44511.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43362.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36756.00</t>
   </si>
 </sst>
 </file>
@@ -464,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,16 +537,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -509,16 +554,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -526,16 +571,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -543,16 +588,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -560,16 +605,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -577,16 +622,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -594,16 +639,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -611,16 +656,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -628,16 +673,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -645,16 +690,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -662,16 +707,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -679,16 +724,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -696,16 +741,16 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -713,16 +758,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -730,16 +775,84 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
-        <v>30</v>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organizando colunas - Arrumando saida de Bases - Arrumando para não sobrepor base temp
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.vinicius\Documents\Vscode\Fipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BCACC7-9318-4429-B041-406060A0964A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F02956-241B-4DF3-B65E-33C4DF158556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="235">
   <si>
     <t>Marca</t>
   </si>
@@ -529,6 +540,207 @@
   </si>
   <si>
     <t>007007-6</t>
+  </si>
+  <si>
+    <t>ASTON MARTIN</t>
+  </si>
+  <si>
+    <t>DB12 Coupe 4.0 V8 680cv</t>
+  </si>
+  <si>
+    <t>085018-7</t>
+  </si>
+  <si>
+    <t>KM a Gasolina</t>
+  </si>
+  <si>
+    <t>DB12 Volante 4.0 V8 680cv</t>
+  </si>
+  <si>
+    <t>085019-5</t>
+  </si>
+  <si>
+    <t>DB9 Coupe 6.0 V12 510cv</t>
+  </si>
+  <si>
+    <t>085011-0</t>
+  </si>
+  <si>
+    <t>DB9 Volante 6.0 V12 470cv</t>
+  </si>
+  <si>
+    <t>085006-3</t>
+  </si>
+  <si>
+    <t>DBS Coupe 5.2 V12 725cv</t>
+  </si>
+  <si>
+    <t>085014-4</t>
+  </si>
+  <si>
+    <t>DBX 4.0 V8 550cv</t>
+  </si>
+  <si>
+    <t>085015-2</t>
+  </si>
+  <si>
+    <t>DBX707 4.0 V8 707cv</t>
+  </si>
+  <si>
+    <t>085016-0</t>
+  </si>
+  <si>
+    <t>Rapide 6.0 V12 477cv</t>
+  </si>
+  <si>
+    <t>085007-1</t>
+  </si>
+  <si>
+    <t>Rapide S 6.0 V12 550cv</t>
+  </si>
+  <si>
+    <t>085009-8</t>
+  </si>
+  <si>
+    <t>Vanquish V12 6.0 565cv</t>
+  </si>
+  <si>
+    <t>085010-1</t>
+  </si>
+  <si>
+    <t>Vantage 6.0 V12 510cv</t>
+  </si>
+  <si>
+    <t>085004-7</t>
+  </si>
+  <si>
+    <t>Vantage Coupe 4.7 V8 425cv</t>
+  </si>
+  <si>
+    <t>085002-0</t>
+  </si>
+  <si>
+    <t>Vantage Cupê  4.0 V8 510cv</t>
+  </si>
+  <si>
+    <t>085012-8</t>
+  </si>
+  <si>
+    <t>Vantage Cupê F1 Edition 4.0 V8 535cv</t>
+  </si>
+  <si>
+    <t>085013-6</t>
+  </si>
+  <si>
+    <t>Vantage Roadster 4.7 V8 420cv</t>
+  </si>
+  <si>
+    <t>085003-9</t>
+  </si>
+  <si>
+    <t>Vantage Roadster F1 Edition 4.0 V8 535cv</t>
+  </si>
+  <si>
+    <t>085017-9</t>
+  </si>
+  <si>
+    <t>Vantage S 6.0 V12 565cv</t>
+  </si>
+  <si>
+    <t>085008-0</t>
+  </si>
+  <si>
+    <t>Vantage S Coupe 4.7 V8 430cv</t>
+  </si>
+  <si>
+    <t>085001-2</t>
+  </si>
+  <si>
+    <t>Virage Coupe 6.0 V12 490cv</t>
+  </si>
+  <si>
+    <t>085005-5</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>100 2.8 V6</t>
+  </si>
+  <si>
+    <t>008030-6</t>
+  </si>
+  <si>
+    <t>100 2.8 V6 Avant</t>
+  </si>
+  <si>
+    <t>008076-4</t>
+  </si>
+  <si>
+    <t>100 S-4 2.2 Avant Turbo</t>
+  </si>
+  <si>
+    <t>008031-4</t>
+  </si>
+  <si>
+    <t>80 2.0</t>
+  </si>
+  <si>
+    <t>008001-2</t>
+  </si>
+  <si>
+    <t>80 2.0 Avant</t>
+  </si>
+  <si>
+    <t>008077-2</t>
+  </si>
+  <si>
+    <t>80 2.6/ 2.8</t>
+  </si>
+  <si>
+    <t>008080-2</t>
+  </si>
+  <si>
+    <t>80 2.6/2.8 Avant</t>
+  </si>
+  <si>
+    <t>008002-0</t>
+  </si>
+  <si>
+    <t>80 2.8 Cabriolet</t>
+  </si>
+  <si>
+    <t>008003-9</t>
+  </si>
+  <si>
+    <t>80 S2 Avant</t>
+  </si>
+  <si>
+    <t>008004-7</t>
+  </si>
+  <si>
+    <t>A1 1.4 TFSI 122cv S-tronic 3p</t>
+  </si>
+  <si>
+    <t>008153-1</t>
+  </si>
+  <si>
+    <t>A1 2.0 TFSI Quattro 256cv 3p</t>
+  </si>
+  <si>
+    <t>008177-9</t>
+  </si>
+  <si>
+    <t>A1 Sport 1.4 TFSI 185cv 3p S-tronic</t>
+  </si>
+  <si>
+    <t>008172-8</t>
+  </si>
+  <si>
+    <t>A1 Sport. S Edition 1.4 TFSI 5p S-tronic</t>
+  </si>
+  <si>
+    <t>008210-4</t>
   </si>
 </sst>
 </file>
@@ -872,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G263"/>
+  <dimension ref="A1:G336"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6938,6 +7150,1685 @@
         <v>12</v>
       </c>
     </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>168</v>
+      </c>
+      <c r="B264" t="s">
+        <v>169</v>
+      </c>
+      <c r="C264" t="s">
+        <v>170</v>
+      </c>
+      <c r="D264">
+        <v>3600000</v>
+      </c>
+      <c r="E264" t="s">
+        <v>171</v>
+      </c>
+      <c r="F264" t="s">
+        <v>62</v>
+      </c>
+      <c r="G264" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>168</v>
+      </c>
+      <c r="B265" t="s">
+        <v>169</v>
+      </c>
+      <c r="C265" t="s">
+        <v>170</v>
+      </c>
+      <c r="D265">
+        <v>3228897</v>
+      </c>
+      <c r="E265" t="s">
+        <v>10</v>
+      </c>
+      <c r="F265" t="s">
+        <v>63</v>
+      </c>
+      <c r="G265" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>168</v>
+      </c>
+      <c r="B266" t="s">
+        <v>169</v>
+      </c>
+      <c r="C266" t="s">
+        <v>170</v>
+      </c>
+      <c r="D266">
+        <v>3070680</v>
+      </c>
+      <c r="E266" t="s">
+        <v>10</v>
+      </c>
+      <c r="F266" t="s">
+        <v>64</v>
+      </c>
+      <c r="G266" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>168</v>
+      </c>
+      <c r="B267" t="s">
+        <v>172</v>
+      </c>
+      <c r="C267" t="s">
+        <v>173</v>
+      </c>
+      <c r="D267">
+        <v>3900000</v>
+      </c>
+      <c r="E267" t="s">
+        <v>171</v>
+      </c>
+      <c r="F267" t="s">
+        <v>62</v>
+      </c>
+      <c r="G267" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>168</v>
+      </c>
+      <c r="B268" t="s">
+        <v>172</v>
+      </c>
+      <c r="C268" t="s">
+        <v>173</v>
+      </c>
+      <c r="D268">
+        <v>3625334</v>
+      </c>
+      <c r="E268" t="s">
+        <v>10</v>
+      </c>
+      <c r="F268" t="s">
+        <v>63</v>
+      </c>
+      <c r="G268" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>168</v>
+      </c>
+      <c r="B269" t="s">
+        <v>174</v>
+      </c>
+      <c r="C269" t="s">
+        <v>175</v>
+      </c>
+      <c r="D269">
+        <v>1214247</v>
+      </c>
+      <c r="E269" t="s">
+        <v>10</v>
+      </c>
+      <c r="F269" t="s">
+        <v>56</v>
+      </c>
+      <c r="G269" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>168</v>
+      </c>
+      <c r="B270" t="s">
+        <v>174</v>
+      </c>
+      <c r="C270" t="s">
+        <v>175</v>
+      </c>
+      <c r="D270">
+        <v>946995</v>
+      </c>
+      <c r="E270" t="s">
+        <v>10</v>
+      </c>
+      <c r="F270" t="s">
+        <v>35</v>
+      </c>
+      <c r="G270" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>168</v>
+      </c>
+      <c r="B271" t="s">
+        <v>176</v>
+      </c>
+      <c r="C271" t="s">
+        <v>177</v>
+      </c>
+      <c r="D271">
+        <v>617791</v>
+      </c>
+      <c r="E271" t="s">
+        <v>10</v>
+      </c>
+      <c r="F271" t="s">
+        <v>38</v>
+      </c>
+      <c r="G271" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>168</v>
+      </c>
+      <c r="B272" t="s">
+        <v>178</v>
+      </c>
+      <c r="C272" t="s">
+        <v>179</v>
+      </c>
+      <c r="D272">
+        <v>4493874</v>
+      </c>
+      <c r="E272" t="s">
+        <v>10</v>
+      </c>
+      <c r="F272" t="s">
+        <v>65</v>
+      </c>
+      <c r="G272" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>168</v>
+      </c>
+      <c r="B273" t="s">
+        <v>178</v>
+      </c>
+      <c r="C273" t="s">
+        <v>179</v>
+      </c>
+      <c r="D273">
+        <v>4142252</v>
+      </c>
+      <c r="E273" t="s">
+        <v>10</v>
+      </c>
+      <c r="F273" t="s">
+        <v>50</v>
+      </c>
+      <c r="G273" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>168</v>
+      </c>
+      <c r="B274" t="s">
+        <v>180</v>
+      </c>
+      <c r="C274" t="s">
+        <v>181</v>
+      </c>
+      <c r="D274">
+        <v>2346605</v>
+      </c>
+      <c r="E274" t="s">
+        <v>10</v>
+      </c>
+      <c r="F274" t="s">
+        <v>65</v>
+      </c>
+      <c r="G274" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>168</v>
+      </c>
+      <c r="B275" t="s">
+        <v>180</v>
+      </c>
+      <c r="C275" t="s">
+        <v>181</v>
+      </c>
+      <c r="D275">
+        <v>2055673</v>
+      </c>
+      <c r="E275" t="s">
+        <v>10</v>
+      </c>
+      <c r="F275" t="s">
+        <v>50</v>
+      </c>
+      <c r="G275" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>168</v>
+      </c>
+      <c r="B276" t="s">
+        <v>182</v>
+      </c>
+      <c r="C276" t="s">
+        <v>183</v>
+      </c>
+      <c r="D276">
+        <v>3800000</v>
+      </c>
+      <c r="E276" t="s">
+        <v>171</v>
+      </c>
+      <c r="F276" t="s">
+        <v>62</v>
+      </c>
+      <c r="G276" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>168</v>
+      </c>
+      <c r="B277" t="s">
+        <v>182</v>
+      </c>
+      <c r="C277" t="s">
+        <v>183</v>
+      </c>
+      <c r="D277">
+        <v>3226068</v>
+      </c>
+      <c r="E277" t="s">
+        <v>10</v>
+      </c>
+      <c r="F277" t="s">
+        <v>63</v>
+      </c>
+      <c r="G277" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>168</v>
+      </c>
+      <c r="B278" t="s">
+        <v>182</v>
+      </c>
+      <c r="C278" t="s">
+        <v>183</v>
+      </c>
+      <c r="D278">
+        <v>2729902</v>
+      </c>
+      <c r="E278" t="s">
+        <v>10</v>
+      </c>
+      <c r="F278" t="s">
+        <v>64</v>
+      </c>
+      <c r="G278" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>168</v>
+      </c>
+      <c r="B279" t="s">
+        <v>182</v>
+      </c>
+      <c r="C279" t="s">
+        <v>183</v>
+      </c>
+      <c r="D279">
+        <v>2502679</v>
+      </c>
+      <c r="E279" t="s">
+        <v>10</v>
+      </c>
+      <c r="F279" t="s">
+        <v>65</v>
+      </c>
+      <c r="G279" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>168</v>
+      </c>
+      <c r="B280" t="s">
+        <v>184</v>
+      </c>
+      <c r="C280" t="s">
+        <v>185</v>
+      </c>
+      <c r="D280">
+        <v>694217</v>
+      </c>
+      <c r="E280" t="s">
+        <v>10</v>
+      </c>
+      <c r="F280" t="s">
+        <v>37</v>
+      </c>
+      <c r="G280" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>168</v>
+      </c>
+      <c r="B281" t="s">
+        <v>184</v>
+      </c>
+      <c r="C281" t="s">
+        <v>185</v>
+      </c>
+      <c r="D281">
+        <v>607011</v>
+      </c>
+      <c r="E281" t="s">
+        <v>10</v>
+      </c>
+      <c r="F281" t="s">
+        <v>38</v>
+      </c>
+      <c r="G281" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>168</v>
+      </c>
+      <c r="B282" t="s">
+        <v>186</v>
+      </c>
+      <c r="C282" t="s">
+        <v>187</v>
+      </c>
+      <c r="D282">
+        <v>1296696</v>
+      </c>
+      <c r="E282" t="s">
+        <v>10</v>
+      </c>
+      <c r="F282" t="s">
+        <v>56</v>
+      </c>
+      <c r="G282" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>168</v>
+      </c>
+      <c r="B283" t="s">
+        <v>186</v>
+      </c>
+      <c r="C283" t="s">
+        <v>187</v>
+      </c>
+      <c r="D283">
+        <v>1032188</v>
+      </c>
+      <c r="E283" t="s">
+        <v>10</v>
+      </c>
+      <c r="F283" t="s">
+        <v>35</v>
+      </c>
+      <c r="G283" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>168</v>
+      </c>
+      <c r="B284" t="s">
+        <v>188</v>
+      </c>
+      <c r="C284" t="s">
+        <v>189</v>
+      </c>
+      <c r="D284">
+        <v>1784133</v>
+      </c>
+      <c r="E284" t="s">
+        <v>10</v>
+      </c>
+      <c r="F284" t="s">
+        <v>56</v>
+      </c>
+      <c r="G284" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>168</v>
+      </c>
+      <c r="B285" t="s">
+        <v>188</v>
+      </c>
+      <c r="C285" t="s">
+        <v>189</v>
+      </c>
+      <c r="D285">
+        <v>1616174</v>
+      </c>
+      <c r="E285" t="s">
+        <v>10</v>
+      </c>
+      <c r="F285" t="s">
+        <v>35</v>
+      </c>
+      <c r="G285" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>168</v>
+      </c>
+      <c r="B286" t="s">
+        <v>190</v>
+      </c>
+      <c r="C286" t="s">
+        <v>191</v>
+      </c>
+      <c r="D286">
+        <v>476063</v>
+      </c>
+      <c r="E286" t="s">
+        <v>10</v>
+      </c>
+      <c r="F286" t="s">
+        <v>37</v>
+      </c>
+      <c r="G286" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>168</v>
+      </c>
+      <c r="B287" t="s">
+        <v>192</v>
+      </c>
+      <c r="C287" t="s">
+        <v>193</v>
+      </c>
+      <c r="D287">
+        <v>638283</v>
+      </c>
+      <c r="E287" t="s">
+        <v>10</v>
+      </c>
+      <c r="F287" t="s">
+        <v>56</v>
+      </c>
+      <c r="G287" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>168</v>
+      </c>
+      <c r="B288" t="s">
+        <v>192</v>
+      </c>
+      <c r="C288" t="s">
+        <v>193</v>
+      </c>
+      <c r="D288">
+        <v>591028</v>
+      </c>
+      <c r="E288" t="s">
+        <v>10</v>
+      </c>
+      <c r="F288" t="s">
+        <v>35</v>
+      </c>
+      <c r="G288" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>168</v>
+      </c>
+      <c r="B289" t="s">
+        <v>192</v>
+      </c>
+      <c r="C289" t="s">
+        <v>193</v>
+      </c>
+      <c r="D289">
+        <v>528207</v>
+      </c>
+      <c r="E289" t="s">
+        <v>10</v>
+      </c>
+      <c r="F289" t="s">
+        <v>37</v>
+      </c>
+      <c r="G289" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>168</v>
+      </c>
+      <c r="B290" t="s">
+        <v>192</v>
+      </c>
+      <c r="C290" t="s">
+        <v>193</v>
+      </c>
+      <c r="D290">
+        <v>515323</v>
+      </c>
+      <c r="E290" t="s">
+        <v>10</v>
+      </c>
+      <c r="F290" t="s">
+        <v>38</v>
+      </c>
+      <c r="G290" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>168</v>
+      </c>
+      <c r="B291" t="s">
+        <v>194</v>
+      </c>
+      <c r="C291" t="s">
+        <v>195</v>
+      </c>
+      <c r="D291">
+        <v>2800750</v>
+      </c>
+      <c r="E291" t="s">
+        <v>171</v>
+      </c>
+      <c r="F291" t="s">
+        <v>62</v>
+      </c>
+      <c r="G291" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>168</v>
+      </c>
+      <c r="B292" t="s">
+        <v>194</v>
+      </c>
+      <c r="C292" t="s">
+        <v>195</v>
+      </c>
+      <c r="D292">
+        <v>2200329</v>
+      </c>
+      <c r="E292" t="s">
+        <v>10</v>
+      </c>
+      <c r="F292" t="s">
+        <v>63</v>
+      </c>
+      <c r="G292" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>168</v>
+      </c>
+      <c r="B293" t="s">
+        <v>194</v>
+      </c>
+      <c r="C293" t="s">
+        <v>195</v>
+      </c>
+      <c r="D293">
+        <v>1739268</v>
+      </c>
+      <c r="E293" t="s">
+        <v>10</v>
+      </c>
+      <c r="F293" t="s">
+        <v>65</v>
+      </c>
+      <c r="G293" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>168</v>
+      </c>
+      <c r="B294" t="s">
+        <v>194</v>
+      </c>
+      <c r="C294" t="s">
+        <v>195</v>
+      </c>
+      <c r="D294">
+        <v>1647750</v>
+      </c>
+      <c r="E294" t="s">
+        <v>10</v>
+      </c>
+      <c r="F294" t="s">
+        <v>50</v>
+      </c>
+      <c r="G294" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>168</v>
+      </c>
+      <c r="B295" t="s">
+        <v>196</v>
+      </c>
+      <c r="C295" t="s">
+        <v>197</v>
+      </c>
+      <c r="D295">
+        <v>1770690</v>
+      </c>
+      <c r="E295" t="s">
+        <v>10</v>
+      </c>
+      <c r="F295" t="s">
+        <v>65</v>
+      </c>
+      <c r="G295" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>168</v>
+      </c>
+      <c r="B296" t="s">
+        <v>196</v>
+      </c>
+      <c r="C296" t="s">
+        <v>197</v>
+      </c>
+      <c r="D296">
+        <v>1706250</v>
+      </c>
+      <c r="E296" t="s">
+        <v>10</v>
+      </c>
+      <c r="F296" t="s">
+        <v>50</v>
+      </c>
+      <c r="G296" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>168</v>
+      </c>
+      <c r="B297" t="s">
+        <v>198</v>
+      </c>
+      <c r="C297" t="s">
+        <v>199</v>
+      </c>
+      <c r="D297">
+        <v>588516</v>
+      </c>
+      <c r="E297" t="s">
+        <v>10</v>
+      </c>
+      <c r="F297" t="s">
+        <v>38</v>
+      </c>
+      <c r="G297" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>168</v>
+      </c>
+      <c r="B298" t="s">
+        <v>198</v>
+      </c>
+      <c r="C298" t="s">
+        <v>199</v>
+      </c>
+      <c r="D298">
+        <v>521625</v>
+      </c>
+      <c r="E298" t="s">
+        <v>10</v>
+      </c>
+      <c r="F298" t="s">
+        <v>39</v>
+      </c>
+      <c r="G298" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>168</v>
+      </c>
+      <c r="B299" t="s">
+        <v>200</v>
+      </c>
+      <c r="C299" t="s">
+        <v>201</v>
+      </c>
+      <c r="D299">
+        <v>1842750</v>
+      </c>
+      <c r="E299" t="s">
+        <v>10</v>
+      </c>
+      <c r="F299" t="s">
+        <v>65</v>
+      </c>
+      <c r="G299" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>168</v>
+      </c>
+      <c r="B300" t="s">
+        <v>202</v>
+      </c>
+      <c r="C300" t="s">
+        <v>203</v>
+      </c>
+      <c r="D300">
+        <v>1145906</v>
+      </c>
+      <c r="E300" t="s">
+        <v>10</v>
+      </c>
+      <c r="F300" t="s">
+        <v>56</v>
+      </c>
+      <c r="G300" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>168</v>
+      </c>
+      <c r="B301" t="s">
+        <v>202</v>
+      </c>
+      <c r="C301" t="s">
+        <v>203</v>
+      </c>
+      <c r="D301">
+        <v>993822</v>
+      </c>
+      <c r="E301" t="s">
+        <v>10</v>
+      </c>
+      <c r="F301" t="s">
+        <v>34</v>
+      </c>
+      <c r="G301" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>168</v>
+      </c>
+      <c r="B302" t="s">
+        <v>204</v>
+      </c>
+      <c r="C302" t="s">
+        <v>205</v>
+      </c>
+      <c r="D302">
+        <v>531136</v>
+      </c>
+      <c r="E302" t="s">
+        <v>10</v>
+      </c>
+      <c r="F302" t="s">
+        <v>37</v>
+      </c>
+      <c r="G302" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>168</v>
+      </c>
+      <c r="B303" t="s">
+        <v>206</v>
+      </c>
+      <c r="C303" t="s">
+        <v>207</v>
+      </c>
+      <c r="D303">
+        <v>654552</v>
+      </c>
+      <c r="E303" t="s">
+        <v>10</v>
+      </c>
+      <c r="F303" t="s">
+        <v>37</v>
+      </c>
+      <c r="G303" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>208</v>
+      </c>
+      <c r="B304" t="s">
+        <v>209</v>
+      </c>
+      <c r="C304" t="s">
+        <v>210</v>
+      </c>
+      <c r="D304">
+        <v>12940</v>
+      </c>
+      <c r="E304" t="s">
+        <v>10</v>
+      </c>
+      <c r="F304" t="s">
+        <v>19</v>
+      </c>
+      <c r="G304" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>208</v>
+      </c>
+      <c r="B305" t="s">
+        <v>209</v>
+      </c>
+      <c r="C305" t="s">
+        <v>210</v>
+      </c>
+      <c r="D305">
+        <v>12146</v>
+      </c>
+      <c r="E305" t="s">
+        <v>10</v>
+      </c>
+      <c r="F305" t="s">
+        <v>20</v>
+      </c>
+      <c r="G305" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>208</v>
+      </c>
+      <c r="B306" t="s">
+        <v>209</v>
+      </c>
+      <c r="C306" t="s">
+        <v>210</v>
+      </c>
+      <c r="D306">
+        <v>10344</v>
+      </c>
+      <c r="E306" t="s">
+        <v>10</v>
+      </c>
+      <c r="F306" t="s">
+        <v>21</v>
+      </c>
+      <c r="G306" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>208</v>
+      </c>
+      <c r="B307" t="s">
+        <v>211</v>
+      </c>
+      <c r="C307" t="s">
+        <v>212</v>
+      </c>
+      <c r="D307">
+        <v>13652</v>
+      </c>
+      <c r="E307" t="s">
+        <v>10</v>
+      </c>
+      <c r="F307" t="s">
+        <v>19</v>
+      </c>
+      <c r="G307" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>208</v>
+      </c>
+      <c r="B308" t="s">
+        <v>211</v>
+      </c>
+      <c r="C308" t="s">
+        <v>212</v>
+      </c>
+      <c r="D308">
+        <v>12238</v>
+      </c>
+      <c r="E308" t="s">
+        <v>10</v>
+      </c>
+      <c r="F308" t="s">
+        <v>20</v>
+      </c>
+      <c r="G308" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>208</v>
+      </c>
+      <c r="B309" t="s">
+        <v>213</v>
+      </c>
+      <c r="C309" t="s">
+        <v>214</v>
+      </c>
+      <c r="D309">
+        <v>23715</v>
+      </c>
+      <c r="E309" t="s">
+        <v>10</v>
+      </c>
+      <c r="F309" t="s">
+        <v>19</v>
+      </c>
+      <c r="G309" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>208</v>
+      </c>
+      <c r="B310" t="s">
+        <v>213</v>
+      </c>
+      <c r="C310" t="s">
+        <v>214</v>
+      </c>
+      <c r="D310">
+        <v>21449</v>
+      </c>
+      <c r="E310" t="s">
+        <v>10</v>
+      </c>
+      <c r="F310" t="s">
+        <v>20</v>
+      </c>
+      <c r="G310" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>208</v>
+      </c>
+      <c r="B311" t="s">
+        <v>215</v>
+      </c>
+      <c r="C311" t="s">
+        <v>216</v>
+      </c>
+      <c r="D311">
+        <v>14965</v>
+      </c>
+      <c r="E311" t="s">
+        <v>10</v>
+      </c>
+      <c r="F311" t="s">
+        <v>19</v>
+      </c>
+      <c r="G311" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>208</v>
+      </c>
+      <c r="B312" t="s">
+        <v>215</v>
+      </c>
+      <c r="C312" t="s">
+        <v>216</v>
+      </c>
+      <c r="D312">
+        <v>12435</v>
+      </c>
+      <c r="E312" t="s">
+        <v>10</v>
+      </c>
+      <c r="F312" t="s">
+        <v>20</v>
+      </c>
+      <c r="G312" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>208</v>
+      </c>
+      <c r="B313" t="s">
+        <v>217</v>
+      </c>
+      <c r="C313" t="s">
+        <v>218</v>
+      </c>
+      <c r="D313">
+        <v>15117</v>
+      </c>
+      <c r="E313" t="s">
+        <v>10</v>
+      </c>
+      <c r="F313" t="s">
+        <v>19</v>
+      </c>
+      <c r="G313" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>208</v>
+      </c>
+      <c r="B314" t="s">
+        <v>217</v>
+      </c>
+      <c r="C314" t="s">
+        <v>218</v>
+      </c>
+      <c r="D314">
+        <v>12483</v>
+      </c>
+      <c r="E314" t="s">
+        <v>10</v>
+      </c>
+      <c r="F314" t="s">
+        <v>20</v>
+      </c>
+      <c r="G314" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>208</v>
+      </c>
+      <c r="B315" t="s">
+        <v>219</v>
+      </c>
+      <c r="C315" t="s">
+        <v>220</v>
+      </c>
+      <c r="D315">
+        <v>23449</v>
+      </c>
+      <c r="E315" t="s">
+        <v>10</v>
+      </c>
+      <c r="F315" t="s">
+        <v>19</v>
+      </c>
+      <c r="G315" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>208</v>
+      </c>
+      <c r="B316" t="s">
+        <v>219</v>
+      </c>
+      <c r="C316" t="s">
+        <v>220</v>
+      </c>
+      <c r="D316">
+        <v>19050</v>
+      </c>
+      <c r="E316" t="s">
+        <v>10</v>
+      </c>
+      <c r="F316" t="s">
+        <v>20</v>
+      </c>
+      <c r="G316" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>208</v>
+      </c>
+      <c r="B317" t="s">
+        <v>221</v>
+      </c>
+      <c r="C317" t="s">
+        <v>222</v>
+      </c>
+      <c r="D317">
+        <v>30297</v>
+      </c>
+      <c r="E317" t="s">
+        <v>10</v>
+      </c>
+      <c r="F317" t="s">
+        <v>18</v>
+      </c>
+      <c r="G317" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>208</v>
+      </c>
+      <c r="B318" t="s">
+        <v>221</v>
+      </c>
+      <c r="C318" t="s">
+        <v>222</v>
+      </c>
+      <c r="D318">
+        <v>29558</v>
+      </c>
+      <c r="E318" t="s">
+        <v>10</v>
+      </c>
+      <c r="F318" t="s">
+        <v>19</v>
+      </c>
+      <c r="G318" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>208</v>
+      </c>
+      <c r="B319" t="s">
+        <v>221</v>
+      </c>
+      <c r="C319" t="s">
+        <v>222</v>
+      </c>
+      <c r="D319">
+        <v>22679</v>
+      </c>
+      <c r="E319" t="s">
+        <v>10</v>
+      </c>
+      <c r="F319" t="s">
+        <v>20</v>
+      </c>
+      <c r="G319" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>208</v>
+      </c>
+      <c r="B320" t="s">
+        <v>223</v>
+      </c>
+      <c r="C320" t="s">
+        <v>224</v>
+      </c>
+      <c r="D320">
+        <v>69220</v>
+      </c>
+      <c r="E320" t="s">
+        <v>10</v>
+      </c>
+      <c r="F320" t="s">
+        <v>85</v>
+      </c>
+      <c r="G320" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>208</v>
+      </c>
+      <c r="B321" t="s">
+        <v>223</v>
+      </c>
+      <c r="C321" t="s">
+        <v>224</v>
+      </c>
+      <c r="D321">
+        <v>67531</v>
+      </c>
+      <c r="E321" t="s">
+        <v>10</v>
+      </c>
+      <c r="F321" t="s">
+        <v>16</v>
+      </c>
+      <c r="G321" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>208</v>
+      </c>
+      <c r="B322" t="s">
+        <v>223</v>
+      </c>
+      <c r="C322" t="s">
+        <v>224</v>
+      </c>
+      <c r="D322">
+        <v>65883</v>
+      </c>
+      <c r="E322" t="s">
+        <v>10</v>
+      </c>
+      <c r="F322" t="s">
+        <v>17</v>
+      </c>
+      <c r="G322" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>208</v>
+      </c>
+      <c r="B323" t="s">
+        <v>223</v>
+      </c>
+      <c r="C323" t="s">
+        <v>224</v>
+      </c>
+      <c r="D323">
+        <v>64276</v>
+      </c>
+      <c r="E323" t="s">
+        <v>10</v>
+      </c>
+      <c r="F323" t="s">
+        <v>18</v>
+      </c>
+      <c r="G323" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>208</v>
+      </c>
+      <c r="B324" t="s">
+        <v>223</v>
+      </c>
+      <c r="C324" t="s">
+        <v>224</v>
+      </c>
+      <c r="D324">
+        <v>62708</v>
+      </c>
+      <c r="E324" t="s">
+        <v>10</v>
+      </c>
+      <c r="F324" t="s">
+        <v>19</v>
+      </c>
+      <c r="G324" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>208</v>
+      </c>
+      <c r="B325" t="s">
+        <v>223</v>
+      </c>
+      <c r="C325" t="s">
+        <v>224</v>
+      </c>
+      <c r="D325">
+        <v>56940</v>
+      </c>
+      <c r="E325" t="s">
+        <v>10</v>
+      </c>
+      <c r="F325" t="s">
+        <v>20</v>
+      </c>
+      <c r="G325" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>208</v>
+      </c>
+      <c r="B326" t="s">
+        <v>225</v>
+      </c>
+      <c r="C326" t="s">
+        <v>226</v>
+      </c>
+      <c r="D326">
+        <v>23516</v>
+      </c>
+      <c r="E326" t="s">
+        <v>10</v>
+      </c>
+      <c r="F326" t="s">
+        <v>19</v>
+      </c>
+      <c r="G326" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>208</v>
+      </c>
+      <c r="B327" t="s">
+        <v>225</v>
+      </c>
+      <c r="C327" t="s">
+        <v>226</v>
+      </c>
+      <c r="D327">
+        <v>19107</v>
+      </c>
+      <c r="E327" t="s">
+        <v>10</v>
+      </c>
+      <c r="F327" t="s">
+        <v>20</v>
+      </c>
+      <c r="G327" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>208</v>
+      </c>
+      <c r="B328" t="s">
+        <v>227</v>
+      </c>
+      <c r="C328" t="s">
+        <v>228</v>
+      </c>
+      <c r="D328">
+        <v>69227</v>
+      </c>
+      <c r="E328" t="s">
+        <v>10</v>
+      </c>
+      <c r="F328" t="s">
+        <v>35</v>
+      </c>
+      <c r="G328" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>208</v>
+      </c>
+      <c r="B329" t="s">
+        <v>227</v>
+      </c>
+      <c r="C329" t="s">
+        <v>228</v>
+      </c>
+      <c r="D329">
+        <v>67538</v>
+      </c>
+      <c r="E329" t="s">
+        <v>10</v>
+      </c>
+      <c r="F329" t="s">
+        <v>36</v>
+      </c>
+      <c r="G329" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>208</v>
+      </c>
+      <c r="B330" t="s">
+        <v>227</v>
+      </c>
+      <c r="C330" t="s">
+        <v>228</v>
+      </c>
+      <c r="D330">
+        <v>58794</v>
+      </c>
+      <c r="E330" t="s">
+        <v>10</v>
+      </c>
+      <c r="F330" t="s">
+        <v>37</v>
+      </c>
+      <c r="G330" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>208</v>
+      </c>
+      <c r="B331" t="s">
+        <v>227</v>
+      </c>
+      <c r="C331" t="s">
+        <v>228</v>
+      </c>
+      <c r="D331">
+        <v>57172</v>
+      </c>
+      <c r="E331" t="s">
+        <v>10</v>
+      </c>
+      <c r="F331" t="s">
+        <v>38</v>
+      </c>
+      <c r="G331" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>208</v>
+      </c>
+      <c r="B332" t="s">
+        <v>229</v>
+      </c>
+      <c r="C332" t="s">
+        <v>230</v>
+      </c>
+      <c r="D332">
+        <v>121907</v>
+      </c>
+      <c r="E332" t="s">
+        <v>10</v>
+      </c>
+      <c r="F332" t="s">
+        <v>36</v>
+      </c>
+      <c r="G332" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>208</v>
+      </c>
+      <c r="B333" t="s">
+        <v>231</v>
+      </c>
+      <c r="C333" t="s">
+        <v>232</v>
+      </c>
+      <c r="D333">
+        <v>73953</v>
+      </c>
+      <c r="E333" t="s">
+        <v>10</v>
+      </c>
+      <c r="F333" t="s">
+        <v>35</v>
+      </c>
+      <c r="G333" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>208</v>
+      </c>
+      <c r="B334" t="s">
+        <v>231</v>
+      </c>
+      <c r="C334" t="s">
+        <v>232</v>
+      </c>
+      <c r="D334">
+        <v>67755</v>
+      </c>
+      <c r="E334" t="s">
+        <v>10</v>
+      </c>
+      <c r="F334" t="s">
+        <v>36</v>
+      </c>
+      <c r="G334" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>208</v>
+      </c>
+      <c r="B335" t="s">
+        <v>231</v>
+      </c>
+      <c r="C335" t="s">
+        <v>232</v>
+      </c>
+      <c r="D335">
+        <v>59243</v>
+      </c>
+      <c r="E335" t="s">
+        <v>10</v>
+      </c>
+      <c r="F335" t="s">
+        <v>37</v>
+      </c>
+      <c r="G335" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>208</v>
+      </c>
+      <c r="B336" t="s">
+        <v>233</v>
+      </c>
+      <c r="C336" t="s">
+        <v>234</v>
+      </c>
+      <c r="D336">
+        <v>82917</v>
+      </c>
+      <c r="E336" t="s">
+        <v>10</v>
+      </c>
+      <c r="F336" t="s">
+        <v>55</v>
+      </c>
+      <c r="G336" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adaptado código para pegar caminhões - Agora falta testar
</commit_message>
<xml_diff>
--- a/Fipe.xlsx
+++ b/Fipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.vinicius\Documents\Vscode\Fipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394B54B3-D208-42B7-B0E3-BF816649F31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9874A6D9-747A-419D-8B2F-09E820C3B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="264">
   <si>
     <t>Marca</t>
   </si>
@@ -756,6 +756,78 @@
   </si>
   <si>
     <t>008204-0</t>
+  </si>
+  <si>
+    <t>A3 1.6 3p</t>
+  </si>
+  <si>
+    <t>008032-2</t>
+  </si>
+  <si>
+    <t>A3 1.6 3p Aut.</t>
+  </si>
+  <si>
+    <t>008056-0</t>
+  </si>
+  <si>
+    <t>A3 1.6 5p</t>
+  </si>
+  <si>
+    <t>008040-3</t>
+  </si>
+  <si>
+    <t>A3 1.6 5p Aut.</t>
+  </si>
+  <si>
+    <t>008057-8</t>
+  </si>
+  <si>
+    <t>A3 1.6 8V 102cv 3p</t>
+  </si>
+  <si>
+    <t>008116-7</t>
+  </si>
+  <si>
+    <t>A3 1.8 3p</t>
+  </si>
+  <si>
+    <t>008005-5</t>
+  </si>
+  <si>
+    <t>A3 1.8 3p Aut.</t>
+  </si>
+  <si>
+    <t>008043-8</t>
+  </si>
+  <si>
+    <t>A3 1.8 5p Aut.</t>
+  </si>
+  <si>
+    <t>008042-0</t>
+  </si>
+  <si>
+    <t>A3 1.8 5p Mec.</t>
+  </si>
+  <si>
+    <t>008041-1</t>
+  </si>
+  <si>
+    <t>A3 1.8 Turbo 180cv 3p Aut./ Tip.</t>
+  </si>
+  <si>
+    <t>008073-0</t>
+  </si>
+  <si>
+    <t>A3 1.8 Turbo 180cv 3p Mec.</t>
+  </si>
+  <si>
+    <t>008074-8</t>
+  </si>
+  <si>
+    <t>A3 1.8 Turbo 180cv 5p Aut./ Tip.</t>
+  </si>
+  <si>
+    <t>008071-3</t>
   </si>
 </sst>
 </file>
@@ -1099,15 +1171,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G347"/>
+  <dimension ref="A1:G421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="H297" sqref="H297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -7178,6 +7250,9 @@
       <c r="D264">
         <v>3600000</v>
       </c>
+      <c r="E264" t="s">
+        <v>10</v>
+      </c>
       <c r="F264" t="s">
         <v>62</v>
       </c>
@@ -7244,6 +7319,9 @@
       <c r="D267">
         <v>3900000</v>
       </c>
+      <c r="E267" t="s">
+        <v>10</v>
+      </c>
       <c r="F267" t="s">
         <v>62</v>
       </c>
@@ -7448,6 +7526,9 @@
       <c r="D276">
         <v>3800000</v>
       </c>
+      <c r="E276" t="s">
+        <v>10</v>
+      </c>
       <c r="F276" t="s">
         <v>62</v>
       </c>
@@ -7790,6 +7871,9 @@
       <c r="D291">
         <v>2800750</v>
       </c>
+      <c r="E291" t="s">
+        <v>10</v>
+      </c>
       <c r="F291" t="s">
         <v>62</v>
       </c>
@@ -9082,6 +9166,1708 @@
         <v>54</v>
       </c>
       <c r="G347" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>207</v>
+      </c>
+      <c r="B348" t="s">
+        <v>238</v>
+      </c>
+      <c r="C348" t="s">
+        <v>239</v>
+      </c>
+      <c r="D348">
+        <v>116902</v>
+      </c>
+      <c r="E348" t="s">
+        <v>10</v>
+      </c>
+      <c r="F348" t="s">
+        <v>55</v>
+      </c>
+      <c r="G348" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>207</v>
+      </c>
+      <c r="B349" t="s">
+        <v>238</v>
+      </c>
+      <c r="C349" t="s">
+        <v>239</v>
+      </c>
+      <c r="D349">
+        <v>107141</v>
+      </c>
+      <c r="E349" t="s">
+        <v>10</v>
+      </c>
+      <c r="F349" t="s">
+        <v>56</v>
+      </c>
+      <c r="G349" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>207</v>
+      </c>
+      <c r="B350" t="s">
+        <v>240</v>
+      </c>
+      <c r="C350" t="s">
+        <v>241</v>
+      </c>
+      <c r="D350">
+        <v>19755</v>
+      </c>
+      <c r="E350" t="s">
+        <v>10</v>
+      </c>
+      <c r="F350" t="s">
+        <v>94</v>
+      </c>
+      <c r="G350" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>207</v>
+      </c>
+      <c r="B351" t="s">
+        <v>240</v>
+      </c>
+      <c r="C351" t="s">
+        <v>241</v>
+      </c>
+      <c r="D351">
+        <v>18974</v>
+      </c>
+      <c r="E351" t="s">
+        <v>10</v>
+      </c>
+      <c r="F351" t="s">
+        <v>103</v>
+      </c>
+      <c r="G351" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>207</v>
+      </c>
+      <c r="B352" t="s">
+        <v>240</v>
+      </c>
+      <c r="C352" t="s">
+        <v>241</v>
+      </c>
+      <c r="D352">
+        <v>18511</v>
+      </c>
+      <c r="E352" t="s">
+        <v>10</v>
+      </c>
+      <c r="F352" t="s">
+        <v>104</v>
+      </c>
+      <c r="G352" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>207</v>
+      </c>
+      <c r="B353" t="s">
+        <v>240</v>
+      </c>
+      <c r="C353" t="s">
+        <v>241</v>
+      </c>
+      <c r="D353">
+        <v>16245</v>
+      </c>
+      <c r="E353" t="s">
+        <v>10</v>
+      </c>
+      <c r="F353" t="s">
+        <v>109</v>
+      </c>
+      <c r="G353" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>207</v>
+      </c>
+      <c r="B354" t="s">
+        <v>240</v>
+      </c>
+      <c r="C354" t="s">
+        <v>241</v>
+      </c>
+      <c r="D354">
+        <v>15235</v>
+      </c>
+      <c r="E354" t="s">
+        <v>10</v>
+      </c>
+      <c r="F354" t="s">
+        <v>85</v>
+      </c>
+      <c r="G354" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>207</v>
+      </c>
+      <c r="B355" t="s">
+        <v>242</v>
+      </c>
+      <c r="C355" t="s">
+        <v>243</v>
+      </c>
+      <c r="D355">
+        <v>21354</v>
+      </c>
+      <c r="E355" t="s">
+        <v>10</v>
+      </c>
+      <c r="F355" t="s">
+        <v>94</v>
+      </c>
+      <c r="G355" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>207</v>
+      </c>
+      <c r="B356" t="s">
+        <v>242</v>
+      </c>
+      <c r="C356" t="s">
+        <v>243</v>
+      </c>
+      <c r="D356">
+        <v>20443</v>
+      </c>
+      <c r="E356" t="s">
+        <v>10</v>
+      </c>
+      <c r="F356" t="s">
+        <v>103</v>
+      </c>
+      <c r="G356" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>207</v>
+      </c>
+      <c r="B357" t="s">
+        <v>242</v>
+      </c>
+      <c r="C357" t="s">
+        <v>243</v>
+      </c>
+      <c r="D357">
+        <v>19315</v>
+      </c>
+      <c r="E357" t="s">
+        <v>10</v>
+      </c>
+      <c r="F357" t="s">
+        <v>104</v>
+      </c>
+      <c r="G357" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>207</v>
+      </c>
+      <c r="B358" t="s">
+        <v>242</v>
+      </c>
+      <c r="C358" t="s">
+        <v>243</v>
+      </c>
+      <c r="D358">
+        <v>16389</v>
+      </c>
+      <c r="E358" t="s">
+        <v>10</v>
+      </c>
+      <c r="F358" t="s">
+        <v>109</v>
+      </c>
+      <c r="G358" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>207</v>
+      </c>
+      <c r="B359" t="s">
+        <v>242</v>
+      </c>
+      <c r="C359" t="s">
+        <v>243</v>
+      </c>
+      <c r="D359">
+        <v>15482</v>
+      </c>
+      <c r="E359" t="s">
+        <v>10</v>
+      </c>
+      <c r="F359" t="s">
+        <v>85</v>
+      </c>
+      <c r="G359" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>207</v>
+      </c>
+      <c r="B360" t="s">
+        <v>244</v>
+      </c>
+      <c r="C360" t="s">
+        <v>245</v>
+      </c>
+      <c r="D360">
+        <v>28210</v>
+      </c>
+      <c r="E360" t="s">
+        <v>10</v>
+      </c>
+      <c r="F360" t="s">
+        <v>29</v>
+      </c>
+      <c r="G360" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>207</v>
+      </c>
+      <c r="B361" t="s">
+        <v>244</v>
+      </c>
+      <c r="C361" t="s">
+        <v>245</v>
+      </c>
+      <c r="D361">
+        <v>26539</v>
+      </c>
+      <c r="E361" t="s">
+        <v>10</v>
+      </c>
+      <c r="F361" t="s">
+        <v>30</v>
+      </c>
+      <c r="G361" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>207</v>
+      </c>
+      <c r="B362" t="s">
+        <v>244</v>
+      </c>
+      <c r="C362" t="s">
+        <v>245</v>
+      </c>
+      <c r="D362">
+        <v>23062</v>
+      </c>
+      <c r="E362" t="s">
+        <v>10</v>
+      </c>
+      <c r="F362" t="s">
+        <v>31</v>
+      </c>
+      <c r="G362" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>207</v>
+      </c>
+      <c r="B363" t="s">
+        <v>244</v>
+      </c>
+      <c r="C363" t="s">
+        <v>245</v>
+      </c>
+      <c r="D363">
+        <v>22499</v>
+      </c>
+      <c r="E363" t="s">
+        <v>10</v>
+      </c>
+      <c r="F363" t="s">
+        <v>94</v>
+      </c>
+      <c r="G363" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>207</v>
+      </c>
+      <c r="B364" t="s">
+        <v>244</v>
+      </c>
+      <c r="C364" t="s">
+        <v>245</v>
+      </c>
+      <c r="D364">
+        <v>20267</v>
+      </c>
+      <c r="E364" t="s">
+        <v>10</v>
+      </c>
+      <c r="F364" t="s">
+        <v>103</v>
+      </c>
+      <c r="G364" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>207</v>
+      </c>
+      <c r="B365" t="s">
+        <v>244</v>
+      </c>
+      <c r="C365" t="s">
+        <v>245</v>
+      </c>
+      <c r="D365">
+        <v>19467</v>
+      </c>
+      <c r="E365" t="s">
+        <v>10</v>
+      </c>
+      <c r="F365" t="s">
+        <v>104</v>
+      </c>
+      <c r="G365" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>207</v>
+      </c>
+      <c r="B366" t="s">
+        <v>244</v>
+      </c>
+      <c r="C366" t="s">
+        <v>245</v>
+      </c>
+      <c r="D366">
+        <v>17989</v>
+      </c>
+      <c r="E366" t="s">
+        <v>10</v>
+      </c>
+      <c r="F366" t="s">
+        <v>109</v>
+      </c>
+      <c r="G366" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>207</v>
+      </c>
+      <c r="B367" t="s">
+        <v>244</v>
+      </c>
+      <c r="C367" t="s">
+        <v>245</v>
+      </c>
+      <c r="D367">
+        <v>16792</v>
+      </c>
+      <c r="E367" t="s">
+        <v>10</v>
+      </c>
+      <c r="F367" t="s">
+        <v>85</v>
+      </c>
+      <c r="G367" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>207</v>
+      </c>
+      <c r="B368" t="s">
+        <v>246</v>
+      </c>
+      <c r="C368" t="s">
+        <v>247</v>
+      </c>
+      <c r="D368">
+        <v>27532</v>
+      </c>
+      <c r="E368" t="s">
+        <v>10</v>
+      </c>
+      <c r="F368" t="s">
+        <v>94</v>
+      </c>
+      <c r="G368" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>207</v>
+      </c>
+      <c r="B369" t="s">
+        <v>246</v>
+      </c>
+      <c r="C369" t="s">
+        <v>247</v>
+      </c>
+      <c r="D369">
+        <v>26860</v>
+      </c>
+      <c r="E369" t="s">
+        <v>10</v>
+      </c>
+      <c r="F369" t="s">
+        <v>103</v>
+      </c>
+      <c r="G369" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>207</v>
+      </c>
+      <c r="B370" t="s">
+        <v>246</v>
+      </c>
+      <c r="C370" t="s">
+        <v>247</v>
+      </c>
+      <c r="D370">
+        <v>25756</v>
+      </c>
+      <c r="E370" t="s">
+        <v>10</v>
+      </c>
+      <c r="F370" t="s">
+        <v>104</v>
+      </c>
+      <c r="G370" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>207</v>
+      </c>
+      <c r="B371" t="s">
+        <v>246</v>
+      </c>
+      <c r="C371" t="s">
+        <v>247</v>
+      </c>
+      <c r="D371">
+        <v>19966</v>
+      </c>
+      <c r="E371" t="s">
+        <v>10</v>
+      </c>
+      <c r="F371" t="s">
+        <v>109</v>
+      </c>
+      <c r="G371" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>207</v>
+      </c>
+      <c r="B372" t="s">
+        <v>246</v>
+      </c>
+      <c r="C372" t="s">
+        <v>247</v>
+      </c>
+      <c r="D372">
+        <v>17486</v>
+      </c>
+      <c r="E372" t="s">
+        <v>10</v>
+      </c>
+      <c r="F372" t="s">
+        <v>85</v>
+      </c>
+      <c r="G372" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>207</v>
+      </c>
+      <c r="B373" t="s">
+        <v>248</v>
+      </c>
+      <c r="C373" t="s">
+        <v>249</v>
+      </c>
+      <c r="D373">
+        <v>34924</v>
+      </c>
+      <c r="E373" t="s">
+        <v>10</v>
+      </c>
+      <c r="F373" t="s">
+        <v>28</v>
+      </c>
+      <c r="G373" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>207</v>
+      </c>
+      <c r="B374" t="s">
+        <v>250</v>
+      </c>
+      <c r="C374" t="s">
+        <v>251</v>
+      </c>
+      <c r="D374">
+        <v>23670</v>
+      </c>
+      <c r="E374" t="s">
+        <v>10</v>
+      </c>
+      <c r="F374" t="s">
+        <v>31</v>
+      </c>
+      <c r="G374" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>207</v>
+      </c>
+      <c r="B375" t="s">
+        <v>250</v>
+      </c>
+      <c r="C375" t="s">
+        <v>251</v>
+      </c>
+      <c r="D375">
+        <v>21307</v>
+      </c>
+      <c r="E375" t="s">
+        <v>10</v>
+      </c>
+      <c r="F375" t="s">
+        <v>94</v>
+      </c>
+      <c r="G375" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>207</v>
+      </c>
+      <c r="B376" t="s">
+        <v>250</v>
+      </c>
+      <c r="C376" t="s">
+        <v>251</v>
+      </c>
+      <c r="D376">
+        <v>20787</v>
+      </c>
+      <c r="E376" t="s">
+        <v>10</v>
+      </c>
+      <c r="F376" t="s">
+        <v>103</v>
+      </c>
+      <c r="G376" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>207</v>
+      </c>
+      <c r="B377" t="s">
+        <v>250</v>
+      </c>
+      <c r="C377" t="s">
+        <v>251</v>
+      </c>
+      <c r="D377">
+        <v>19054</v>
+      </c>
+      <c r="E377" t="s">
+        <v>10</v>
+      </c>
+      <c r="F377" t="s">
+        <v>104</v>
+      </c>
+      <c r="G377" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>207</v>
+      </c>
+      <c r="B378" t="s">
+        <v>250</v>
+      </c>
+      <c r="C378" t="s">
+        <v>251</v>
+      </c>
+      <c r="D378">
+        <v>18588</v>
+      </c>
+      <c r="E378" t="s">
+        <v>10</v>
+      </c>
+      <c r="F378" t="s">
+        <v>109</v>
+      </c>
+      <c r="G378" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>207</v>
+      </c>
+      <c r="B379" t="s">
+        <v>250</v>
+      </c>
+      <c r="C379" t="s">
+        <v>251</v>
+      </c>
+      <c r="D379">
+        <v>17671</v>
+      </c>
+      <c r="E379" t="s">
+        <v>10</v>
+      </c>
+      <c r="F379" t="s">
+        <v>85</v>
+      </c>
+      <c r="G379" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>207</v>
+      </c>
+      <c r="B380" t="s">
+        <v>250</v>
+      </c>
+      <c r="C380" t="s">
+        <v>251</v>
+      </c>
+      <c r="D380">
+        <v>17210</v>
+      </c>
+      <c r="E380" t="s">
+        <v>10</v>
+      </c>
+      <c r="F380" t="s">
+        <v>16</v>
+      </c>
+      <c r="G380" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>207</v>
+      </c>
+      <c r="B381" t="s">
+        <v>250</v>
+      </c>
+      <c r="C381" t="s">
+        <v>251</v>
+      </c>
+      <c r="D381">
+        <v>16522</v>
+      </c>
+      <c r="E381" t="s">
+        <v>10</v>
+      </c>
+      <c r="F381" t="s">
+        <v>17</v>
+      </c>
+      <c r="G381" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>207</v>
+      </c>
+      <c r="B382" t="s">
+        <v>252</v>
+      </c>
+      <c r="C382" t="s">
+        <v>253</v>
+      </c>
+      <c r="D382">
+        <v>24304</v>
+      </c>
+      <c r="E382" t="s">
+        <v>10</v>
+      </c>
+      <c r="F382" t="s">
+        <v>31</v>
+      </c>
+      <c r="G382" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>207</v>
+      </c>
+      <c r="B383" t="s">
+        <v>252</v>
+      </c>
+      <c r="C383" t="s">
+        <v>253</v>
+      </c>
+      <c r="D383">
+        <v>22150</v>
+      </c>
+      <c r="E383" t="s">
+        <v>10</v>
+      </c>
+      <c r="F383" t="s">
+        <v>94</v>
+      </c>
+      <c r="G383" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>207</v>
+      </c>
+      <c r="B384" t="s">
+        <v>252</v>
+      </c>
+      <c r="C384" t="s">
+        <v>253</v>
+      </c>
+      <c r="D384">
+        <v>20880</v>
+      </c>
+      <c r="E384" t="s">
+        <v>10</v>
+      </c>
+      <c r="F384" t="s">
+        <v>103</v>
+      </c>
+      <c r="G384" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>207</v>
+      </c>
+      <c r="B385" t="s">
+        <v>252</v>
+      </c>
+      <c r="C385" t="s">
+        <v>253</v>
+      </c>
+      <c r="D385">
+        <v>19384</v>
+      </c>
+      <c r="E385" t="s">
+        <v>10</v>
+      </c>
+      <c r="F385" t="s">
+        <v>104</v>
+      </c>
+      <c r="G385" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>207</v>
+      </c>
+      <c r="B386" t="s">
+        <v>252</v>
+      </c>
+      <c r="C386" t="s">
+        <v>253</v>
+      </c>
+      <c r="D386">
+        <v>18590</v>
+      </c>
+      <c r="E386" t="s">
+        <v>10</v>
+      </c>
+      <c r="F386" t="s">
+        <v>109</v>
+      </c>
+      <c r="G386" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>207</v>
+      </c>
+      <c r="B387" t="s">
+        <v>252</v>
+      </c>
+      <c r="C387" t="s">
+        <v>253</v>
+      </c>
+      <c r="D387">
+        <v>18054</v>
+      </c>
+      <c r="E387" t="s">
+        <v>10</v>
+      </c>
+      <c r="F387" t="s">
+        <v>85</v>
+      </c>
+      <c r="G387" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>207</v>
+      </c>
+      <c r="B388" t="s">
+        <v>252</v>
+      </c>
+      <c r="C388" t="s">
+        <v>253</v>
+      </c>
+      <c r="D388">
+        <v>17269</v>
+      </c>
+      <c r="E388" t="s">
+        <v>10</v>
+      </c>
+      <c r="F388" t="s">
+        <v>16</v>
+      </c>
+      <c r="G388" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>207</v>
+      </c>
+      <c r="B389" t="s">
+        <v>252</v>
+      </c>
+      <c r="C389" t="s">
+        <v>253</v>
+      </c>
+      <c r="D389">
+        <v>16685</v>
+      </c>
+      <c r="E389" t="s">
+        <v>10</v>
+      </c>
+      <c r="F389" t="s">
+        <v>17</v>
+      </c>
+      <c r="G389" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>207</v>
+      </c>
+      <c r="B390" t="s">
+        <v>254</v>
+      </c>
+      <c r="C390" t="s">
+        <v>255</v>
+      </c>
+      <c r="D390">
+        <v>29127</v>
+      </c>
+      <c r="E390" t="s">
+        <v>10</v>
+      </c>
+      <c r="F390" t="s">
+        <v>29</v>
+      </c>
+      <c r="G390" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>207</v>
+      </c>
+      <c r="B391" t="s">
+        <v>254</v>
+      </c>
+      <c r="C391" t="s">
+        <v>255</v>
+      </c>
+      <c r="D391">
+        <v>28389</v>
+      </c>
+      <c r="E391" t="s">
+        <v>10</v>
+      </c>
+      <c r="F391" t="s">
+        <v>30</v>
+      </c>
+      <c r="G391" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>207</v>
+      </c>
+      <c r="B392" t="s">
+        <v>254</v>
+      </c>
+      <c r="C392" t="s">
+        <v>255</v>
+      </c>
+      <c r="D392">
+        <v>27696</v>
+      </c>
+      <c r="E392" t="s">
+        <v>10</v>
+      </c>
+      <c r="F392" t="s">
+        <v>31</v>
+      </c>
+      <c r="G392" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>207</v>
+      </c>
+      <c r="B393" t="s">
+        <v>254</v>
+      </c>
+      <c r="C393" t="s">
+        <v>255</v>
+      </c>
+      <c r="D393">
+        <v>25740</v>
+      </c>
+      <c r="E393" t="s">
+        <v>10</v>
+      </c>
+      <c r="F393" t="s">
+        <v>94</v>
+      </c>
+      <c r="G393" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>207</v>
+      </c>
+      <c r="B394" t="s">
+        <v>254</v>
+      </c>
+      <c r="C394" t="s">
+        <v>255</v>
+      </c>
+      <c r="D394">
+        <v>22881</v>
+      </c>
+      <c r="E394" t="s">
+        <v>10</v>
+      </c>
+      <c r="F394" t="s">
+        <v>103</v>
+      </c>
+      <c r="G394" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>207</v>
+      </c>
+      <c r="B395" t="s">
+        <v>254</v>
+      </c>
+      <c r="C395" t="s">
+        <v>255</v>
+      </c>
+      <c r="D395">
+        <v>21584</v>
+      </c>
+      <c r="E395" t="s">
+        <v>10</v>
+      </c>
+      <c r="F395" t="s">
+        <v>104</v>
+      </c>
+      <c r="G395" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>207</v>
+      </c>
+      <c r="B396" t="s">
+        <v>254</v>
+      </c>
+      <c r="C396" t="s">
+        <v>255</v>
+      </c>
+      <c r="D396">
+        <v>19616</v>
+      </c>
+      <c r="E396" t="s">
+        <v>10</v>
+      </c>
+      <c r="F396" t="s">
+        <v>109</v>
+      </c>
+      <c r="G396" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>207</v>
+      </c>
+      <c r="B397" t="s">
+        <v>254</v>
+      </c>
+      <c r="C397" t="s">
+        <v>255</v>
+      </c>
+      <c r="D397">
+        <v>19137</v>
+      </c>
+      <c r="E397" t="s">
+        <v>10</v>
+      </c>
+      <c r="F397" t="s">
+        <v>85</v>
+      </c>
+      <c r="G397" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>207</v>
+      </c>
+      <c r="B398" t="s">
+        <v>254</v>
+      </c>
+      <c r="C398" t="s">
+        <v>255</v>
+      </c>
+      <c r="D398">
+        <v>17310</v>
+      </c>
+      <c r="E398" t="s">
+        <v>10</v>
+      </c>
+      <c r="F398" t="s">
+        <v>16</v>
+      </c>
+      <c r="G398" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>207</v>
+      </c>
+      <c r="B399" t="s">
+        <v>254</v>
+      </c>
+      <c r="C399" t="s">
+        <v>255</v>
+      </c>
+      <c r="D399">
+        <v>16711</v>
+      </c>
+      <c r="E399" t="s">
+        <v>10</v>
+      </c>
+      <c r="F399" t="s">
+        <v>17</v>
+      </c>
+      <c r="G399" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>207</v>
+      </c>
+      <c r="B400" t="s">
+        <v>256</v>
+      </c>
+      <c r="C400" t="s">
+        <v>257</v>
+      </c>
+      <c r="D400">
+        <v>26439</v>
+      </c>
+      <c r="E400" t="s">
+        <v>10</v>
+      </c>
+      <c r="F400" t="s">
+        <v>29</v>
+      </c>
+      <c r="G400" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>207</v>
+      </c>
+      <c r="B401" t="s">
+        <v>256</v>
+      </c>
+      <c r="C401" t="s">
+        <v>257</v>
+      </c>
+      <c r="D401">
+        <v>25794</v>
+      </c>
+      <c r="E401" t="s">
+        <v>10</v>
+      </c>
+      <c r="F401" t="s">
+        <v>30</v>
+      </c>
+      <c r="G401" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>207</v>
+      </c>
+      <c r="B402" t="s">
+        <v>256</v>
+      </c>
+      <c r="C402" t="s">
+        <v>257</v>
+      </c>
+      <c r="D402">
+        <v>23944</v>
+      </c>
+      <c r="E402" t="s">
+        <v>10</v>
+      </c>
+      <c r="F402" t="s">
+        <v>31</v>
+      </c>
+      <c r="G402" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>207</v>
+      </c>
+      <c r="B403" t="s">
+        <v>256</v>
+      </c>
+      <c r="C403" t="s">
+        <v>257</v>
+      </c>
+      <c r="D403">
+        <v>22551</v>
+      </c>
+      <c r="E403" t="s">
+        <v>10</v>
+      </c>
+      <c r="F403" t="s">
+        <v>94</v>
+      </c>
+      <c r="G403" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>207</v>
+      </c>
+      <c r="B404" t="s">
+        <v>256</v>
+      </c>
+      <c r="C404" t="s">
+        <v>257</v>
+      </c>
+      <c r="D404">
+        <v>21669</v>
+      </c>
+      <c r="E404" t="s">
+        <v>10</v>
+      </c>
+      <c r="F404" t="s">
+        <v>103</v>
+      </c>
+      <c r="G404" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>207</v>
+      </c>
+      <c r="B405" t="s">
+        <v>256</v>
+      </c>
+      <c r="C405" t="s">
+        <v>257</v>
+      </c>
+      <c r="D405">
+        <v>20926</v>
+      </c>
+      <c r="E405" t="s">
+        <v>10</v>
+      </c>
+      <c r="F405" t="s">
+        <v>104</v>
+      </c>
+      <c r="G405" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>207</v>
+      </c>
+      <c r="B406" t="s">
+        <v>256</v>
+      </c>
+      <c r="C406" t="s">
+        <v>257</v>
+      </c>
+      <c r="D406">
+        <v>18963</v>
+      </c>
+      <c r="E406" t="s">
+        <v>10</v>
+      </c>
+      <c r="F406" t="s">
+        <v>109</v>
+      </c>
+      <c r="G406" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>207</v>
+      </c>
+      <c r="B407" t="s">
+        <v>256</v>
+      </c>
+      <c r="C407" t="s">
+        <v>257</v>
+      </c>
+      <c r="D407">
+        <v>18051</v>
+      </c>
+      <c r="E407" t="s">
+        <v>10</v>
+      </c>
+      <c r="F407" t="s">
+        <v>85</v>
+      </c>
+      <c r="G407" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>207</v>
+      </c>
+      <c r="B408" t="s">
+        <v>256</v>
+      </c>
+      <c r="C408" t="s">
+        <v>257</v>
+      </c>
+      <c r="D408">
+        <v>17265</v>
+      </c>
+      <c r="E408" t="s">
+        <v>10</v>
+      </c>
+      <c r="F408" t="s">
+        <v>16</v>
+      </c>
+      <c r="G408" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>207</v>
+      </c>
+      <c r="B409" t="s">
+        <v>256</v>
+      </c>
+      <c r="C409" t="s">
+        <v>257</v>
+      </c>
+      <c r="D409">
+        <v>16694</v>
+      </c>
+      <c r="E409" t="s">
+        <v>10</v>
+      </c>
+      <c r="F409" t="s">
+        <v>17</v>
+      </c>
+      <c r="G409" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>207</v>
+      </c>
+      <c r="B410" t="s">
+        <v>258</v>
+      </c>
+      <c r="C410" t="s">
+        <v>259</v>
+      </c>
+      <c r="D410">
+        <v>26714</v>
+      </c>
+      <c r="E410" t="s">
+        <v>10</v>
+      </c>
+      <c r="F410" t="s">
+        <v>94</v>
+      </c>
+      <c r="G410" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>207</v>
+      </c>
+      <c r="B411" t="s">
+        <v>258</v>
+      </c>
+      <c r="C411" t="s">
+        <v>259</v>
+      </c>
+      <c r="D411">
+        <v>21512</v>
+      </c>
+      <c r="E411" t="s">
+        <v>10</v>
+      </c>
+      <c r="F411" t="s">
+        <v>103</v>
+      </c>
+      <c r="G411" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>207</v>
+      </c>
+      <c r="B412" t="s">
+        <v>260</v>
+      </c>
+      <c r="C412" t="s">
+        <v>261</v>
+      </c>
+      <c r="D412">
+        <v>23754</v>
+      </c>
+      <c r="E412" t="s">
+        <v>10</v>
+      </c>
+      <c r="F412" t="s">
+        <v>31</v>
+      </c>
+      <c r="G412" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>207</v>
+      </c>
+      <c r="B413" t="s">
+        <v>260</v>
+      </c>
+      <c r="C413" t="s">
+        <v>261</v>
+      </c>
+      <c r="D413">
+        <v>22346</v>
+      </c>
+      <c r="E413" t="s">
+        <v>10</v>
+      </c>
+      <c r="F413" t="s">
+        <v>94</v>
+      </c>
+      <c r="G413" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>207</v>
+      </c>
+      <c r="B414" t="s">
+        <v>260</v>
+      </c>
+      <c r="C414" t="s">
+        <v>261</v>
+      </c>
+      <c r="D414">
+        <v>20556</v>
+      </c>
+      <c r="E414" t="s">
+        <v>10</v>
+      </c>
+      <c r="F414" t="s">
+        <v>103</v>
+      </c>
+      <c r="G414" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>207</v>
+      </c>
+      <c r="B415" t="s">
+        <v>260</v>
+      </c>
+      <c r="C415" t="s">
+        <v>261</v>
+      </c>
+      <c r="D415">
+        <v>17333</v>
+      </c>
+      <c r="E415" t="s">
+        <v>10</v>
+      </c>
+      <c r="F415" t="s">
+        <v>104</v>
+      </c>
+      <c r="G415" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>207</v>
+      </c>
+      <c r="B416" t="s">
+        <v>260</v>
+      </c>
+      <c r="C416" t="s">
+        <v>261</v>
+      </c>
+      <c r="D416">
+        <v>16910</v>
+      </c>
+      <c r="E416" t="s">
+        <v>10</v>
+      </c>
+      <c r="F416" t="s">
+        <v>109</v>
+      </c>
+      <c r="G416" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>207</v>
+      </c>
+      <c r="B417" t="s">
+        <v>262</v>
+      </c>
+      <c r="C417" t="s">
+        <v>263</v>
+      </c>
+      <c r="D417">
+        <v>39909</v>
+      </c>
+      <c r="E417" t="s">
+        <v>10</v>
+      </c>
+      <c r="F417" t="s">
+        <v>29</v>
+      </c>
+      <c r="G417" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>207</v>
+      </c>
+      <c r="B418" t="s">
+        <v>262</v>
+      </c>
+      <c r="C418" t="s">
+        <v>263</v>
+      </c>
+      <c r="D418">
+        <v>34183</v>
+      </c>
+      <c r="E418" t="s">
+        <v>10</v>
+      </c>
+      <c r="F418" t="s">
+        <v>30</v>
+      </c>
+      <c r="G418" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>207</v>
+      </c>
+      <c r="B419" t="s">
+        <v>262</v>
+      </c>
+      <c r="C419" t="s">
+        <v>263</v>
+      </c>
+      <c r="D419">
+        <v>27982</v>
+      </c>
+      <c r="E419" t="s">
+        <v>10</v>
+      </c>
+      <c r="F419" t="s">
+        <v>31</v>
+      </c>
+      <c r="G419" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>207</v>
+      </c>
+      <c r="B420" t="s">
+        <v>262</v>
+      </c>
+      <c r="C420" t="s">
+        <v>263</v>
+      </c>
+      <c r="D420">
+        <v>27299</v>
+      </c>
+      <c r="E420" t="s">
+        <v>10</v>
+      </c>
+      <c r="F420" t="s">
+        <v>94</v>
+      </c>
+      <c r="G420" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>207</v>
+      </c>
+      <c r="B421" t="s">
+        <v>262</v>
+      </c>
+      <c r="C421" t="s">
+        <v>263</v>
+      </c>
+      <c r="D421">
+        <v>23657</v>
+      </c>
+      <c r="E421" t="s">
+        <v>10</v>
+      </c>
+      <c r="F421" t="s">
+        <v>103</v>
+      </c>
+      <c r="G421" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>